<commit_message>
working remove from list
</commit_message>
<xml_diff>
--- a/USER GRID.xlsx
+++ b/USER GRID.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14740" tabRatio="500"/>
+    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="14740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="113">
   <si>
     <t>GUEST</t>
   </si>
@@ -154,13 +154,251 @@
   </si>
   <si>
     <t>array of FK of PP</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>image_url</t>
+  </si>
+  <si>
+    <t>what to get</t>
+  </si>
+  <si>
+    <t>Di Fara Pizza</t>
+  </si>
+  <si>
+    <t>neighborhood</t>
+  </si>
+  <si>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>Rubirosa</t>
+  </si>
+  <si>
+    <t>Nolita</t>
+  </si>
+  <si>
+    <t>Classic Pie</t>
+  </si>
+  <si>
+    <t>Keste</t>
+  </si>
+  <si>
+    <t>West Village</t>
+  </si>
+  <si>
+    <t>Margherita</t>
+  </si>
+  <si>
+    <t>Lucali</t>
+  </si>
+  <si>
+    <t>Carroll Gardens</t>
+  </si>
+  <si>
+    <t>Pie with Basil</t>
+  </si>
+  <si>
+    <t>https://media.timeout.com/images/102421883/580/435/image.jpg</t>
+  </si>
+  <si>
+    <t>https://media.timeout.com/images/102421885/580/435/image.jpg</t>
+  </si>
+  <si>
+    <t>https://media.timeout.com/images/102421889/580/435/image.jpg</t>
+  </si>
+  <si>
+    <t>https://media.timeout.com/images/102421891/580/435/image.jpg</t>
+  </si>
+  <si>
+    <t>Totonno's</t>
+  </si>
+  <si>
+    <t>https://media.timeout.com/images/102421893/580/435/image.jpg</t>
+  </si>
+  <si>
+    <t>Franny's</t>
+  </si>
+  <si>
+    <t>Clam Pie</t>
+  </si>
+  <si>
+    <t>https://media.timeout.com/images/100519677/580/435/image.jpg</t>
+  </si>
+  <si>
+    <t>Prospect Heights</t>
+  </si>
+  <si>
+    <t>Margot's</t>
+  </si>
+  <si>
+    <t>Clinton Hill</t>
+  </si>
+  <si>
+    <t>Hot Supreme</t>
+  </si>
+  <si>
+    <t>https://media.timeout.com/images/102421901/580/435/image.jpg</t>
+  </si>
+  <si>
+    <t>Joe's</t>
+  </si>
+  <si>
+    <t>Pepperoni</t>
+  </si>
+  <si>
+    <t>https://media.timeout.com/images/102421899/580/435/image.jpg</t>
+  </si>
+  <si>
+    <t>Patsy's</t>
+  </si>
+  <si>
+    <t>East Harlem</t>
+  </si>
+  <si>
+    <t>https://media.timeout.com/images/100519387/580/435/image.jpg</t>
+  </si>
+  <si>
+    <t>Roberta's</t>
+  </si>
+  <si>
+    <t>Williamsburg</t>
+  </si>
+  <si>
+    <t>Bee Sting</t>
+  </si>
+  <si>
+    <t>https://media.timeout.com/images/100519403/580/435/image.jpg</t>
+  </si>
+  <si>
+    <t>1424 Avenue J, Brooklyn, NY 11230</t>
+  </si>
+  <si>
+    <t>235 Mulberry St, New York, NY 10012</t>
+  </si>
+  <si>
+    <t>271 Bleecker St, New York, NY 10014</t>
+  </si>
+  <si>
+    <t>575 Henry St, New York, NY 11231</t>
+  </si>
+  <si>
+    <t>(718) 258-1367</t>
+  </si>
+  <si>
+    <t>(212) 965-0500</t>
+  </si>
+  <si>
+    <t>(212) 243-1500</t>
+  </si>
+  <si>
+    <t>(718) 858-4086</t>
+  </si>
+  <si>
+    <t>1524 Neptune Ave, Brooklyn, NY 11224</t>
+  </si>
+  <si>
+    <t>(718) 372-8606</t>
+  </si>
+  <si>
+    <t>www.difara.com/</t>
+  </si>
+  <si>
+    <t>www.kestepizzeria.com/</t>
+  </si>
+  <si>
+    <t>www.lucali.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.totonnosconeyisland.com/
+</t>
+  </si>
+  <si>
+    <t>348 Flatbush Ave, Brooklyn, NY 11217</t>
+  </si>
+  <si>
+    <t>(718) 230-0221</t>
+  </si>
+  <si>
+    <r>
+      <t>frannys</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>brooklyn.com/</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">rubirosanyc.com/
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 919 Fulton St, Brooklyn, NY 11238</t>
+  </si>
+  <si>
+    <t>margotspizza.com/</t>
+  </si>
+  <si>
+    <t>7 Carmine St</t>
+  </si>
+  <si>
+    <t>(212) 366 - 1182</t>
+  </si>
+  <si>
+    <t>www.joespizzanyc.com/</t>
+  </si>
+  <si>
+    <t>www.patsys.com/</t>
+  </si>
+  <si>
+    <t>(212) 247-3491</t>
+  </si>
+  <si>
+    <t>236 W 56th St, New York, NY 10019</t>
+  </si>
+  <si>
+    <t>(718) 417-1118</t>
+  </si>
+  <si>
+    <r>
+      <t>www.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>robertas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>pizza.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>261 Moore St, Brooklyn, NY 11206</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -205,6 +443,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF006621"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF006621"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -266,7 +523,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -284,9 +541,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -316,8 +579,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="19"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -326,6 +596,7 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -334,6 +605,8 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -663,15 +936,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" customWidth="1"/>
@@ -679,292 +953,292 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="16" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="D2" s="11"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="3" t="s">
+      <c r="G3" s="9"/>
+      <c r="H3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="19"/>
-      <c r="N3" s="8"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="9"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="F4" s="8" t="s">
+      <c r="D4" s="14"/>
+      <c r="F4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M4" s="19"/>
-      <c r="N4" s="8"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="9"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="F5" s="10"/>
-      <c r="N5" s="7"/>
+      <c r="D5" s="14"/>
+      <c r="F5" s="11"/>
+      <c r="N5" s="8"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="H6" s="2" t="s">
+      <c r="D6" s="14"/>
+      <c r="H6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="5"/>
+      <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="2" t="s">
+      <c r="D7" s="15"/>
+      <c r="E7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F7" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="Q7" s="6"/>
+      <c r="Q7" s="7"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3" t="s">
+      <c r="D8" s="14"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Q8" s="5"/>
+      <c r="Q8" s="6"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="13"/>
+      <c r="D9" s="14"/>
       <c r="N9" t="s">
         <v>37</v>
       </c>
-      <c r="Q9" s="5"/>
+      <c r="Q9" s="6"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="H10" s="2" t="s">
+      <c r="D10" s="14"/>
+      <c r="H10" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="11" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="14"/>
+      <c r="E11" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F11" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="K11" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="11" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="13"/>
+      <c r="D12" s="14"/>
       <c r="F12" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3" t="s">
+      <c r="H12" s="4"/>
+      <c r="I12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -973,7 +1247,265 @@
         <v>43</v>
       </c>
     </row>
+    <row r="18" spans="2:8">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="30">
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="45">
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="H23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="17">
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="G24" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="G26" t="s">
+        <v>76</v>
+      </c>
+      <c r="H26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="F27" t="s">
+        <v>107</v>
+      </c>
+      <c r="G27" t="s">
+        <v>79</v>
+      </c>
+      <c r="H27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="17">
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="G28" t="s">
+        <v>83</v>
+      </c>
+      <c r="H28" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G19" r:id="rId1"/>
+    <hyperlink ref="G20" r:id="rId2"/>
+    <hyperlink ref="G21" r:id="rId3"/>
+    <hyperlink ref="G22" r:id="rId4"/>
+    <hyperlink ref="G23" r:id="rId5"/>
+    <hyperlink ref="F26" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
fixed delete account so only user logged in can see it
</commit_message>
<xml_diff>
--- a/USER GRID.xlsx
+++ b/USER GRID.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="14740" tabRatio="500"/>
+    <workbookView xWindow="1200" yWindow="0" windowWidth="12800" windowHeight="14740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="113">
   <si>
     <t>GUEST</t>
   </si>
@@ -523,7 +523,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -544,6 +544,83 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -587,7 +664,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="97">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -597,6 +674,83 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -938,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1171,9 +1325,6 @@
         <v>7</v>
       </c>
       <c r="D9" s="14"/>
-      <c r="N9" t="s">
-        <v>37</v>
-      </c>
       <c r="Q9" s="6"/>
     </row>
     <row r="10" spans="1:17">

</xml_diff>